<commit_message>
New code for board
</commit_message>
<xml_diff>
--- a/Buttons/Button_List.xlsx
+++ b/Buttons/Button_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ptoth/Documents/Git/A320Overhead/Buttons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9C05EA-A34F-2E47-88AB-5B9A1AB67F58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC46E423-2434-1C43-940A-96AEF8655E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" firstSheet="8" activeTab="9" xr2:uid="{FDAB788E-CCDB-1B47-AE52-300FE5AA462F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="9" xr2:uid="{FDAB788E-CCDB-1B47-AE52-300FE5AA462F}"/>
   </bookViews>
   <sheets>
     <sheet name="Iluminação" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Ar Condicionado'!$A$1:$N$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Board_01_Buttons!$A$1:$D$41</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Elec!$A$1:$N$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Fire!$A$1:$N$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Fuel!$A$1:$N$9</definedName>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2718" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2787" uniqueCount="577">
   <si>
     <t>Codigo do Botão</t>
   </si>
@@ -1763,6 +1764,33 @@
   </si>
   <si>
     <t>LED OUT 08</t>
+  </si>
+  <si>
+    <t>Cod</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Pinout</t>
+  </si>
+  <si>
+    <t>Korry</t>
+  </si>
+  <si>
+    <t>3 Pole</t>
+  </si>
+  <si>
+    <t>2 Pole</t>
+  </si>
+  <si>
+    <t>Analog</t>
+  </si>
+  <si>
+    <t>0-255</t>
+  </si>
+  <si>
+    <t>Códigos Internos / Valores</t>
   </si>
 </sst>
 </file>
@@ -1931,7 +1959,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2020,6 +2048,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2035,6 +2075,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2354,7 +2398,7 @@
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3547,80 +3591,80 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L29" s="31" t="s">
+      <c r="L29" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="M29" s="31"/>
+      <c r="M29" s="35"/>
       <c r="N29" s="3">
         <f>SUMIF(M2:M27,"Digital",N2:N27)</f>
         <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L30" s="31" t="s">
+      <c r="L30" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="M30" s="31"/>
+      <c r="M30" s="35"/>
       <c r="N30" s="3">
         <f>COUNTIF(M2:M27,"Analógico")</f>
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L31" s="31" t="s">
+      <c r="L31" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="M31" s="31"/>
+      <c r="M31" s="35"/>
       <c r="N31" s="3">
         <f>SUM(F2:F27)</f>
         <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L32" s="31" t="s">
+      <c r="L32" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="M32" s="31"/>
+      <c r="M32" s="35"/>
       <c r="N32" s="3">
         <f>COUNTIF(H2:J27, "Azul")</f>
         <v>6</v>
       </c>
     </row>
     <row r="33" spans="12:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L33" s="31" t="s">
+      <c r="L33" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="M33" s="31"/>
+      <c r="M33" s="35"/>
       <c r="N33" s="3">
         <f>COUNTIF(H2:J27, "Laranja")</f>
         <v>6</v>
       </c>
     </row>
     <row r="34" spans="12:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L34" s="31" t="s">
+      <c r="L34" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="M34" s="31"/>
+      <c r="M34" s="35"/>
       <c r="N34" s="3">
         <f>COUNTIF(H2:J27, "Branco")</f>
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="12:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L35" s="31" t="s">
+      <c r="L35" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="M35" s="31"/>
+      <c r="M35" s="35"/>
       <c r="N35" s="3">
         <f>COUNTIF(H2:J27, "Verde")</f>
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="12:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L36" s="31" t="s">
+      <c r="L36" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="M36" s="31"/>
+      <c r="M36" s="35"/>
       <c r="N36" s="3">
         <f>SUM(N32:N35)</f>
         <v>15</v>
@@ -3645,10 +3689,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C1F4B3-22B5-C64A-9DE6-E01F62AC2D3D}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3656,449 +3700,959 @@
     <col min="1" max="1" width="9.83203125" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" customWidth="1"/>
     <col min="3" max="3" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="17">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
+        <v>568</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>569</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>570</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>576</v>
+      </c>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="E2" s="2">
+        <v>100</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>575</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="18">
+      <c r="D3" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
         <v>2</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="G3" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="33">
+        <v>2</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>574</v>
+      </c>
+      <c r="E4" s="33">
+        <v>101</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="33">
+        <v>2</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C5" s="19" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="17">
+      <c r="D5" s="19" t="s">
+        <v>571</v>
+      </c>
+      <c r="E5" s="19">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="F5" s="19">
+        <v>4</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="E6" s="2">
+        <v>102</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>575</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="18">
+      <c r="D7" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="E7" s="8">
+        <v>5</v>
+      </c>
+      <c r="F7" s="8">
+        <v>6</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="33">
         <v>4</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C8" s="19" t="s">
+        <v>474</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>572</v>
+      </c>
+      <c r="E8" s="19">
+        <v>7</v>
+      </c>
+      <c r="F8" s="19">
+        <v>8</v>
+      </c>
+      <c r="G8" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="33">
+        <v>4</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="18">
+      <c r="D9" s="19" t="s">
+        <v>572</v>
+      </c>
+      <c r="E9" s="19">
+        <v>10</v>
+      </c>
+      <c r="F9" s="19">
+        <v>11</v>
+      </c>
+      <c r="G9" s="19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="33">
         <v>4</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B10" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>574</v>
+      </c>
+      <c r="E10" s="33">
+        <v>103</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="G10" s="33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>5</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="E11" s="8">
+        <v>13</v>
+      </c>
+      <c r="F11" s="8">
+        <v>14</v>
+      </c>
+      <c r="G11" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>5</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="E12" s="8">
+        <v>16</v>
+      </c>
+      <c r="F12" s="8">
+        <v>17</v>
+      </c>
+      <c r="G12" s="8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="33">
         <v>6</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="17">
+      <c r="B13" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>477</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>572</v>
+      </c>
+      <c r="E13" s="19">
+        <v>19</v>
+      </c>
+      <c r="F13" s="19">
+        <v>20</v>
+      </c>
+      <c r="G13" s="19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="33">
+        <v>6</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>478</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>572</v>
+      </c>
+      <c r="E14" s="19">
+        <v>22</v>
+      </c>
+      <c r="F14" s="19">
+        <v>23</v>
+      </c>
+      <c r="G14" s="19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>7</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="E15" s="3">
+        <v>25</v>
+      </c>
+      <c r="F15" s="3">
+        <v>26</v>
+      </c>
+      <c r="G15" s="3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>7</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="E16" s="3">
+        <v>28</v>
+      </c>
+      <c r="F16" s="3">
+        <v>29</v>
+      </c>
+      <c r="G16" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="33">
+        <v>8</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>481</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>572</v>
+      </c>
+      <c r="E17" s="19">
+        <v>31</v>
+      </c>
+      <c r="F17" s="19">
+        <v>32</v>
+      </c>
+      <c r="G17" s="19">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="33">
+        <v>8</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>482</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>572</v>
+      </c>
+      <c r="E18" s="19">
+        <v>34</v>
+      </c>
+      <c r="F18" s="19">
+        <v>35</v>
+      </c>
+      <c r="G18" s="19">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>9</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>483</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="E19" s="8">
+        <v>37</v>
+      </c>
+      <c r="F19" s="8">
+        <v>38</v>
+      </c>
+      <c r="G19" s="8">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>9</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="E20" s="8">
+        <v>40</v>
+      </c>
+      <c r="F20" s="8">
+        <v>41</v>
+      </c>
+      <c r="G20" s="8">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="33">
+        <v>10</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>485</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>572</v>
+      </c>
+      <c r="E21" s="19">
+        <v>43</v>
+      </c>
+      <c r="F21" s="19">
+        <v>44</v>
+      </c>
+      <c r="G21" s="19">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="33">
+        <v>10</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>486</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>572</v>
+      </c>
+      <c r="E22" s="19">
+        <v>46</v>
+      </c>
+      <c r="F22" s="19">
+        <v>47</v>
+      </c>
+      <c r="G22" s="19">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>11</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="E23" s="3">
+        <v>49</v>
+      </c>
+      <c r="F23" s="3">
+        <v>50</v>
+      </c>
+      <c r="G23" s="3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>11</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="E24" s="3">
+        <v>52</v>
+      </c>
+      <c r="F24" s="3">
+        <v>53</v>
+      </c>
+      <c r="G24" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="33">
+        <v>12</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>489</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>572</v>
+      </c>
+      <c r="E25" s="20">
+        <v>55</v>
+      </c>
+      <c r="F25" s="20">
+        <v>56</v>
+      </c>
+      <c r="G25" s="20">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="33">
+        <v>12</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>490</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>572</v>
+      </c>
+      <c r="E26" s="20">
+        <v>58</v>
+      </c>
+      <c r="F26" s="20">
+        <v>59</v>
+      </c>
+      <c r="G26" s="20">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>13</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="E27" s="3">
+        <v>61</v>
+      </c>
+      <c r="F27" s="3">
+        <v>62</v>
+      </c>
+      <c r="G27" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>13</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="E28" s="3">
+        <v>64</v>
+      </c>
+      <c r="F28" s="3">
+        <v>65</v>
+      </c>
+      <c r="G28" s="3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="33">
+        <v>14</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>573</v>
+      </c>
+      <c r="E29" s="33">
+        <v>67</v>
+      </c>
+      <c r="F29" s="33">
+        <v>68</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="34">
+        <v>15</v>
+      </c>
+      <c r="B30" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="17">
+      <c r="C30" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>573</v>
+      </c>
+      <c r="E30" s="23">
+        <v>69</v>
+      </c>
+      <c r="F30" s="23">
+        <v>70</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="33">
+        <v>16</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>573</v>
+      </c>
+      <c r="E31" s="33">
+        <v>71</v>
+      </c>
+      <c r="F31" s="33">
+        <v>72</v>
+      </c>
+      <c r="G31" s="33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="34">
+        <v>17</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D32" s="22" t="s">
+        <v>573</v>
+      </c>
+      <c r="E32" s="22">
+        <v>73</v>
+      </c>
+      <c r="F32" s="22">
+        <v>74</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="33">
+        <v>18</v>
+      </c>
+      <c r="B33" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="18">
-        <v>6</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="18">
-        <v>6</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="17">
-        <v>7</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="17">
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="18">
-        <v>8</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="18">
-        <v>8</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="17">
-        <v>9</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="17">
-        <v>9</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="18">
-        <v>10</v>
-      </c>
-      <c r="B16" s="19" t="s">
+      <c r="C33" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>571</v>
+      </c>
+      <c r="E33" s="33">
+        <v>75</v>
+      </c>
+      <c r="F33" s="33">
+        <v>76</v>
+      </c>
+      <c r="G33" s="33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="34">
+        <v>19</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>571</v>
+      </c>
+      <c r="E34" s="22">
+        <v>77</v>
+      </c>
+      <c r="F34" s="22">
+        <v>78</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="33">
+        <v>20</v>
+      </c>
+      <c r="B35" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="D35" s="33" t="s">
+        <v>571</v>
+      </c>
+      <c r="E35" s="33">
+        <v>79</v>
+      </c>
+      <c r="F35" s="33">
+        <v>80</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="34">
         <v>21</v>
       </c>
-      <c r="C16" s="19" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="18">
-        <v>10</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="17">
-        <v>11</v>
-      </c>
-      <c r="B18" s="3" t="s">
+      <c r="B36" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>571</v>
+      </c>
+      <c r="E36" s="22">
+        <v>81</v>
+      </c>
+      <c r="F36" s="22">
+        <v>82</v>
+      </c>
+      <c r="G36" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="33">
         <v>22</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="17">
-        <v>11</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="18">
-        <v>12</v>
-      </c>
-      <c r="B20" s="20" t="s">
+      <c r="B37" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="D37" s="33" t="s">
+        <v>571</v>
+      </c>
+      <c r="E37" s="33">
+        <v>83</v>
+      </c>
+      <c r="F37" s="33">
+        <v>84</v>
+      </c>
+      <c r="G37" s="33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="34">
         <v>23</v>
       </c>
-      <c r="C20" s="20" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="18">
-        <v>12</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="17">
-        <v>13</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="B38" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>571</v>
+      </c>
+      <c r="E38" s="22">
+        <v>85</v>
+      </c>
+      <c r="F38" s="22">
+        <v>86</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="33">
+        <v>24</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="D39" s="33" t="s">
+        <v>571</v>
+      </c>
+      <c r="E39" s="33">
+        <v>87</v>
+      </c>
+      <c r="F39" s="33">
+        <v>88</v>
+      </c>
+      <c r="G39" s="33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="34">
         <v>25</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="18">
-        <v>13</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="17">
-        <v>14</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="18">
-        <v>15</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="17">
-        <v>16</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="18">
-        <v>17</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="17">
-        <v>18</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="18">
+      <c r="B40" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B29" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="17">
-        <v>20</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="18">
-        <v>21</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="17">
-        <v>22</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="18">
-        <v>23</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="17">
+      <c r="C40" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>571</v>
+      </c>
+      <c r="E40" s="22">
+        <v>89</v>
+      </c>
+      <c r="F40" s="22">
+        <v>90</v>
+      </c>
+      <c r="G40" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="33">
+        <v>26</v>
+      </c>
+      <c r="B41" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="18">
-        <v>25</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="17">
-        <v>26</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="C41" s="33" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="27">
-        <v>1</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="29">
-        <v>2</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="29" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="27">
-        <v>3</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="27" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="29">
-        <v>4</v>
-      </c>
-      <c r="B42" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>222</v>
+      <c r="D41" s="33" t="s">
+        <v>571</v>
+      </c>
+      <c r="E41" s="33">
+        <v>91</v>
+      </c>
+      <c r="F41" s="33">
+        <v>92</v>
+      </c>
+      <c r="G41" s="33" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D41" xr:uid="{C7C1F4B3-22B5-C64A-9DE6-E01F62AC2D3D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D41">
+      <sortCondition ref="A1:A41"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="1">
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -8098,11 +8652,11 @@
       <c r="C29" s="23"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="39" t="s">
         <v>508</v>
       </c>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="21"/>
@@ -9605,10 +10159,10 @@
     </row>
     <row r="15" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K15" s="5"/>
-      <c r="L15" s="31" t="s">
+      <c r="L15" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="M15" s="31"/>
+      <c r="M15" s="35"/>
       <c r="N15" s="3">
         <f>SUMIF(M2:M13,"Digital",N2:N13)</f>
         <v>7</v>
@@ -9616,10 +10170,10 @@
     </row>
     <row r="16" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K16" s="5"/>
-      <c r="L16" s="31" t="s">
+      <c r="L16" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="M16" s="31"/>
+      <c r="M16" s="35"/>
       <c r="N16" s="3">
         <f>COUNTIF(M2:M13,"Analógico")</f>
         <v>5</v>
@@ -9627,10 +10181,10 @@
     </row>
     <row r="17" spans="11:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K17" s="5"/>
-      <c r="L17" s="31" t="s">
+      <c r="L17" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="M17" s="31"/>
+      <c r="M17" s="35"/>
       <c r="N17" s="3">
         <f>SUM(F2:F13)</f>
         <v>13</v>
@@ -9638,10 +10192,10 @@
     </row>
     <row r="18" spans="11:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K18" s="5"/>
-      <c r="L18" s="31" t="s">
+      <c r="L18" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="M18" s="31"/>
+      <c r="M18" s="35"/>
       <c r="N18" s="3">
         <f>COUNTIF(H2:J13, "Azul")</f>
         <v>1</v>
@@ -9649,10 +10203,10 @@
     </row>
     <row r="19" spans="11:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K19" s="5"/>
-      <c r="L19" s="31" t="s">
+      <c r="L19" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="M19" s="31"/>
+      <c r="M19" s="35"/>
       <c r="N19" s="3">
         <f>COUNTIF(H2:J13, "Laranja")</f>
         <v>6</v>
@@ -9660,10 +10214,10 @@
     </row>
     <row r="20" spans="11:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K20" s="5"/>
-      <c r="L20" s="31" t="s">
+      <c r="L20" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="M20" s="31"/>
+      <c r="M20" s="35"/>
       <c r="N20" s="3">
         <f>COUNTIF(H2:J13, "Branco")</f>
         <v>6</v>
@@ -9671,10 +10225,10 @@
     </row>
     <row r="21" spans="11:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K21" s="5"/>
-      <c r="L21" s="31" t="s">
+      <c r="L21" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="M21" s="31"/>
+      <c r="M21" s="35"/>
       <c r="N21" s="3">
         <f>SUM(N18:N20)</f>
         <v>13</v>
@@ -10354,10 +10908,10 @@
     </row>
     <row r="16" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K16" s="5"/>
-      <c r="L16" s="32" t="s">
+      <c r="L16" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="M16" s="33"/>
+      <c r="M16" s="37"/>
       <c r="N16" s="7">
         <f>SUMIF(M1:M14,"Digital",N1:N14)</f>
         <v>17</v>
@@ -10365,10 +10919,10 @@
     </row>
     <row r="17" spans="11:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K17" s="5"/>
-      <c r="L17" s="32" t="s">
+      <c r="L17" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="M17" s="33"/>
+      <c r="M17" s="37"/>
       <c r="N17" s="7">
         <f>COUNTIF(M1:M14,"Analógico")</f>
         <v>0</v>
@@ -10376,10 +10930,10 @@
     </row>
     <row r="18" spans="11:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K18" s="5"/>
-      <c r="L18" s="32" t="s">
+      <c r="L18" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="M18" s="33"/>
+      <c r="M18" s="37"/>
       <c r="N18" s="7">
         <f>SUM(F1:F14)</f>
         <v>67</v>
@@ -10387,10 +10941,10 @@
     </row>
     <row r="19" spans="11:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K19" s="5"/>
-      <c r="L19" s="31" t="s">
+      <c r="L19" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="M19" s="31"/>
+      <c r="M19" s="35"/>
       <c r="N19" s="3">
         <f>COUNTIF(H2:J14, "Laranja")</f>
         <v>9</v>
@@ -10398,10 +10952,10 @@
     </row>
     <row r="20" spans="11:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K20" s="5"/>
-      <c r="L20" s="31" t="s">
+      <c r="L20" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="M20" s="31"/>
+      <c r="M20" s="35"/>
       <c r="N20" s="3">
         <f>COUNTIF(H2:J14, "Branco")</f>
         <v>9</v>
@@ -10409,10 +10963,10 @@
     </row>
     <row r="21" spans="11:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K21" s="5"/>
-      <c r="L21" s="31" t="s">
+      <c r="L21" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="M21" s="31"/>
+      <c r="M21" s="35"/>
       <c r="N21" s="3">
         <f>COUNTIF(H2:J14, "Verde")</f>
         <v>1</v>
@@ -10420,10 +10974,10 @@
     </row>
     <row r="22" spans="11:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K22" s="5"/>
-      <c r="L22" s="31" t="s">
+      <c r="L22" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="M22" s="31"/>
+      <c r="M22" s="35"/>
       <c r="N22" s="3">
         <f>SUM(N19:N21)</f>
         <v>19</v>
@@ -10884,10 +11438,10 @@
     </row>
     <row r="11" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K11" s="5"/>
-      <c r="L11" s="31" t="s">
+      <c r="L11" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="M11" s="31"/>
+      <c r="M11" s="35"/>
       <c r="N11" s="3">
         <f>SUMIF(M2:M9,"Digital",N2:N9)</f>
         <v>8</v>
@@ -10895,10 +11449,10 @@
     </row>
     <row r="12" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K12" s="5"/>
-      <c r="L12" s="31" t="s">
+      <c r="L12" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="M12" s="31"/>
+      <c r="M12" s="35"/>
       <c r="N12" s="3">
         <f>COUNTIF(M2:M9,"Analógico")</f>
         <v>0</v>
@@ -10906,10 +11460,10 @@
     </row>
     <row r="13" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K13" s="5"/>
-      <c r="L13" s="31" t="s">
+      <c r="L13" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="M13" s="31"/>
+      <c r="M13" s="35"/>
       <c r="N13" s="3">
         <f>SUM(F2:F9)</f>
         <v>16</v>
@@ -10917,10 +11471,10 @@
     </row>
     <row r="14" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K14" s="5"/>
-      <c r="L14" s="31" t="s">
+      <c r="L14" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="M14" s="31"/>
+      <c r="M14" s="35"/>
       <c r="N14" s="3">
         <f>COUNTIF(H2:J9, "Laranja")</f>
         <v>7</v>
@@ -10928,10 +11482,10 @@
     </row>
     <row r="15" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K15" s="5"/>
-      <c r="L15" s="31" t="s">
+      <c r="L15" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="M15" s="31"/>
+      <c r="M15" s="35"/>
       <c r="N15" s="3">
         <f>COUNTIF(H2:J9, "Branco")</f>
         <v>8</v>
@@ -10939,10 +11493,10 @@
     </row>
     <row r="16" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K16" s="5"/>
-      <c r="L16" s="31" t="s">
+      <c r="L16" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="M16" s="31"/>
+      <c r="M16" s="35"/>
       <c r="N16" s="3">
         <f>COUNTIF(H2:J9, "Verde")</f>
         <v>1</v>
@@ -10950,10 +11504,10 @@
     </row>
     <row r="17" spans="11:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K17" s="5"/>
-      <c r="L17" s="31" t="s">
+      <c r="L17" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="M17" s="31"/>
+      <c r="M17" s="35"/>
       <c r="N17" s="3">
         <f>SUM(N14:N16)</f>
         <v>16</v>
@@ -11350,10 +11904,10 @@
     </row>
     <row r="9" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K9" s="5"/>
-      <c r="L9" s="31" t="s">
+      <c r="L9" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="M9" s="31"/>
+      <c r="M9" s="35"/>
       <c r="N9" s="3">
         <f>SUMIF(M2:M7,"Digital",N2:N7)</f>
         <v>6</v>
@@ -11361,10 +11915,10 @@
     </row>
     <row r="10" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K10" s="5"/>
-      <c r="L10" s="31" t="s">
+      <c r="L10" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="M10" s="31"/>
+      <c r="M10" s="35"/>
       <c r="N10" s="3">
         <f>COUNTIF(M2:M7,"Analógico")</f>
         <v>0</v>
@@ -11372,10 +11926,10 @@
     </row>
     <row r="11" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K11" s="5"/>
-      <c r="L11" s="31" t="s">
+      <c r="L11" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="M11" s="31"/>
+      <c r="M11" s="35"/>
       <c r="N11" s="3">
         <f>SUM(F2:F7)</f>
         <v>11</v>
@@ -11383,10 +11937,10 @@
     </row>
     <row r="12" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K12" s="5"/>
-      <c r="L12" s="31" t="s">
+      <c r="L12" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="M12" s="31"/>
+      <c r="M12" s="35"/>
       <c r="N12" s="3">
         <f>COUNTIF(H2:J7, "Laranja")</f>
         <v>5</v>
@@ -11394,10 +11948,10 @@
     </row>
     <row r="13" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K13" s="5"/>
-      <c r="L13" s="31" t="s">
+      <c r="L13" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="M13" s="31"/>
+      <c r="M13" s="35"/>
       <c r="N13" s="3">
         <f>COUNTIF(H2:J7, "Branco")</f>
         <v>6</v>
@@ -11405,10 +11959,10 @@
     </row>
     <row r="14" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K14" s="5"/>
-      <c r="L14" s="31" t="s">
+      <c r="L14" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="M14" s="31"/>
+      <c r="M14" s="35"/>
       <c r="N14" s="3">
         <f>SUM(N12:N13)</f>
         <v>11</v>
@@ -12010,10 +12564,10 @@
     </row>
     <row r="14" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K14" s="5"/>
-      <c r="L14" s="31" t="s">
+      <c r="L14" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="M14" s="31"/>
+      <c r="M14" s="35"/>
       <c r="N14" s="3">
         <f>SUMIF(M2:M12,"Digital",N2:N12)</f>
         <v>11</v>
@@ -12021,10 +12575,10 @@
     </row>
     <row r="15" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K15" s="5"/>
-      <c r="L15" s="31" t="s">
+      <c r="L15" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="M15" s="31"/>
+      <c r="M15" s="35"/>
       <c r="N15" s="3">
         <f>COUNTIF(M2:M12,"Analógico")</f>
         <v>0</v>
@@ -12032,10 +12586,10 @@
     </row>
     <row r="16" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K16" s="5"/>
-      <c r="L16" s="31" t="s">
+      <c r="L16" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="M16" s="31"/>
+      <c r="M16" s="35"/>
       <c r="N16" s="3">
         <f>SUM(F2:F12)</f>
         <v>37</v>
@@ -12043,10 +12597,10 @@
     </row>
     <row r="17" spans="11:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K17" s="5"/>
-      <c r="L17" s="31" t="s">
+      <c r="L17" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="M17" s="31"/>
+      <c r="M17" s="35"/>
       <c r="N17" s="3">
         <f>COUNTIF(H2:J12, "Laranja")</f>
         <v>5</v>
@@ -12054,10 +12608,10 @@
     </row>
     <row r="18" spans="11:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K18" s="5"/>
-      <c r="L18" s="31" t="s">
+      <c r="L18" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="M18" s="31"/>
+      <c r="M18" s="35"/>
       <c r="N18" s="3">
         <f>COUNTIF(H2:J12,"Branco")</f>
         <v>8</v>
@@ -12065,10 +12619,10 @@
     </row>
     <row r="19" spans="11:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K19" s="5"/>
-      <c r="L19" s="31" t="s">
+      <c r="L19" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="M19" s="31"/>
+      <c r="M19" s="35"/>
       <c r="N19" s="3">
         <f>SUM(F4,F6,F10)</f>
         <v>24</v>
@@ -12076,10 +12630,10 @@
     </row>
     <row r="20" spans="11:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K20" s="5"/>
-      <c r="L20" s="31" t="s">
+      <c r="L20" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="M20" s="31"/>
+      <c r="M20" s="35"/>
       <c r="N20" s="3">
         <f>SUM(N17:N19)</f>
         <v>37</v>
@@ -12962,80 +13516,80 @@
     <row r="20" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K21" s="5"/>
-      <c r="L21" s="31" t="s">
+      <c r="L21" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="M21" s="31"/>
+      <c r="M21" s="35"/>
       <c r="N21" s="3">
         <f>SUMIF(M2:M19,"Digital",N2:N19)</f>
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L22" s="31" t="s">
+      <c r="L22" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="M22" s="31"/>
+      <c r="M22" s="35"/>
       <c r="N22" s="3">
         <f>COUNTIF(M2:M19,"Analógico")</f>
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L23" s="31" t="s">
+      <c r="L23" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="M23" s="31"/>
+      <c r="M23" s="35"/>
       <c r="N23" s="3">
         <f>SUM(F2:F19)</f>
         <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L24" s="31" t="s">
+      <c r="L24" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="M24" s="31"/>
+      <c r="M24" s="35"/>
       <c r="N24" s="3">
         <f>COUNTIF(H2:J19, "Laranja")</f>
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L25" s="31" t="s">
+      <c r="L25" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="M25" s="31"/>
+      <c r="M25" s="35"/>
       <c r="N25" s="3">
         <f>COUNTIF(H2:J19, "Branco")</f>
         <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L26" s="31" t="s">
+      <c r="L26" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="M26" s="31"/>
+      <c r="M26" s="35"/>
       <c r="N26" s="3">
         <f>COUNTIF(H1:J19, "Azul")</f>
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L27" s="31" t="s">
+      <c r="L27" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="M27" s="31"/>
+      <c r="M27" s="35"/>
       <c r="N27" s="3">
         <f>COUNTIF(H2:J19, "Vermelho")</f>
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L28" s="31" t="s">
+      <c r="L28" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="M28" s="31"/>
+      <c r="M28" s="35"/>
       <c r="N28" s="3">
         <f>SUM(N24:N27)</f>
         <v>25</v>
@@ -14711,80 +15265,80 @@
       <c r="B38" s="9"/>
     </row>
     <row r="39" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L39" s="31" t="s">
+      <c r="L39" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="M39" s="31"/>
+      <c r="M39" s="35"/>
       <c r="N39" s="3">
         <f>SUMIF(M2:M37,"Digital",N2:N37)</f>
         <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L40" s="34" t="s">
+      <c r="L40" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="M40" s="34"/>
+      <c r="M40" s="38"/>
       <c r="N40" s="3">
         <f>COUNTIF(M2:M37,"Analógico")</f>
         <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L41" s="34" t="s">
+      <c r="L41" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="M41" s="34"/>
+      <c r="M41" s="38"/>
       <c r="N41" s="3">
         <f>SUM(F2:F37)</f>
         <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L42" s="31" t="s">
+      <c r="L42" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="M42" s="31"/>
+      <c r="M42" s="35"/>
       <c r="N42" s="3">
         <f>COUNTIF(H2:J37, "Laranja")</f>
         <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L43" s="31" t="s">
+      <c r="L43" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="M43" s="31"/>
+      <c r="M43" s="35"/>
       <c r="N43" s="3">
         <f>COUNTIF(H2:J37, "Branco")</f>
         <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L44" s="31" t="s">
+      <c r="L44" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="M44" s="31"/>
+      <c r="M44" s="35"/>
       <c r="N44" s="3">
         <f>COUNTIF(H2:J37, "Azul")</f>
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L45" s="31" t="s">
+      <c r="L45" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="M45" s="31"/>
+      <c r="M45" s="35"/>
       <c r="N45" s="3">
         <f>COUNTIF(H2:J37, "Vermelho")</f>
         <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L46" s="31" t="s">
+      <c r="L46" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="M46" s="31"/>
+      <c r="M46" s="35"/>
       <c r="N46" s="3">
         <f>SUM(N42:N45)</f>
         <v>45</v>

</xml_diff>